<commit_message>
feat: prod - 22 new games
</commit_message>
<xml_diff>
--- a/input/HALL_LIST.xlsx
+++ b/input/HALL_LIST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\open_games\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C058F4-0D87-4E6B-9F16-A5DFFD13A70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C7F4A3-D2B0-4F34-9DEB-CBB8935616B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="313">
   <si>
     <t>Cid</t>
   </si>
@@ -33,457 +33,403 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>ep7DHvTdais5</t>
+    <t>r0CtAXAw5SfD</t>
   </si>
   <si>
     <t>123BET_HALL</t>
   </si>
   <si>
-    <t>O7PtciuTI3MN</t>
+    <t>xQBfOsyQkyh9</t>
   </si>
   <si>
     <t>12IWIN_HALL</t>
   </si>
   <si>
-    <t>jGktKTNCOOsR</t>
+    <t>tLWikh9KAMNV</t>
   </si>
   <si>
     <t>1688_HALL</t>
   </si>
   <si>
-    <t>WMU5idtyNV6p</t>
+    <t>pfqMwQx7gNLj</t>
   </si>
   <si>
     <t>1688IDR_HALL</t>
   </si>
   <si>
-    <t>5ujBeAVfcEeF</t>
+    <t>o40HgoBL2OMy</t>
   </si>
   <si>
     <t>178_HALL</t>
   </si>
   <si>
-    <t>MdISsnN3o1jm</t>
+    <t>3T3DlprkkxlA</t>
   </si>
   <si>
     <t>178S_HALL</t>
   </si>
   <si>
-    <t>2NdppOEAO4rJ</t>
+    <t>NKuRB7GjZXRm</t>
   </si>
   <si>
     <t>1819BET_HALL</t>
   </si>
   <si>
-    <t>14NLVKNeVchr</t>
+    <t>N1rRNQ4Q1W2N</t>
   </si>
   <si>
     <t>1FAZBET_HALL</t>
   </si>
   <si>
-    <t>VNshwCdECBuF</t>
+    <t>nY6Ao0I7snTB</t>
   </si>
   <si>
     <t>2GOALBET_HALL</t>
   </si>
   <si>
-    <t>2NW3VdubPga1</t>
+    <t>WHtrOHu9Ug49</t>
   </si>
   <si>
     <t>2HILO_HALL</t>
   </si>
   <si>
-    <t>d4iF9fa03K5k</t>
+    <t>5Uuqi7ZvnK9x</t>
   </si>
   <si>
     <t>365BETGROUP_HALL</t>
   </si>
   <si>
-    <t>GiyFq7YRc5fL</t>
+    <t>GJhTzUTAMHoL</t>
   </si>
   <si>
     <t>456BETT_HALL</t>
   </si>
   <si>
-    <t>FDo3ZXdRPOo4</t>
+    <t>K2VmPd4wHOAS</t>
   </si>
   <si>
     <t>5GBET_HALL</t>
   </si>
   <si>
-    <t>8fXEc7UNKt4M</t>
+    <t>dBQHjMOSmjjA</t>
   </si>
   <si>
     <t>789BETTING_HALL</t>
   </si>
   <si>
-    <t>NW0h7EBXHT6M</t>
+    <t>CuhKZ1BXdjtR</t>
   </si>
   <si>
     <t>88CASINO_HALL</t>
   </si>
   <si>
-    <t>To5jCj0etzIq</t>
-  </si>
-  <si>
-    <t>9K_HALL</t>
-  </si>
-  <si>
-    <t>2avDTtRxR5FT</t>
-  </si>
-  <si>
-    <t>AB_HALL</t>
-  </si>
-  <si>
-    <t>5qr8FPm1Sd82</t>
+    <t>xEKifQHIUWmF</t>
   </si>
   <si>
     <t>ABCGAME_HALL</t>
   </si>
   <si>
-    <t>pRMfIwAjSU7x</t>
+    <t>9XXd0WwUavVS</t>
   </si>
   <si>
     <t>ALADDINS_HALL</t>
   </si>
   <si>
-    <t>7WIsZZcWQ5KG</t>
+    <t>qck2QrNzmKHb</t>
   </si>
   <si>
     <t>ALFABITZ_HALL</t>
   </si>
   <si>
-    <t>O4rkNSWjLvhx</t>
+    <t>0YX1tHSBSsZJ</t>
   </si>
   <si>
     <t>ALLINGAME_HALL</t>
   </si>
   <si>
-    <t>R8rHEKzrv51M</t>
+    <t>BpWA3XrYtSGE</t>
   </si>
   <si>
     <t>ALLSTAR55_HALL</t>
   </si>
   <si>
-    <t>xBUjsENXibUL</t>
+    <t>Ms5gascD7x3P</t>
   </si>
   <si>
     <t>ALLUREBETS_HALL</t>
   </si>
   <si>
-    <t>HpoHdJ8NutWk</t>
+    <t>nKIXcMZKxfZT</t>
+  </si>
+  <si>
+    <t>AMBBET_HALL</t>
+  </si>
+  <si>
+    <t>2rXP9nmoFxkO</t>
+  </si>
+  <si>
+    <t>AMBET123_HALL</t>
+  </si>
+  <si>
+    <t>WTYeVthpuLUA</t>
+  </si>
+  <si>
+    <t>AMBFUN_HALL</t>
+  </si>
+  <si>
+    <t>Oiv92mnUIB49</t>
+  </si>
+  <si>
+    <t>AMBNEWSPORTB</t>
+  </si>
+  <si>
+    <t>OeIMx1Va8EgF</t>
+  </si>
+  <si>
+    <t>AMBSUPERAPI_HALL</t>
+  </si>
+  <si>
+    <t>uNWjylU9N4lE</t>
+  </si>
+  <si>
+    <t>Ambsuperslot</t>
+  </si>
+  <si>
+    <t>Jiie6xLOgGMK</t>
   </si>
   <si>
     <t>AMB_Hall</t>
   </si>
   <si>
-    <t>pivx9EvjZnVC</t>
-  </si>
-  <si>
-    <t>AMBBET_HALL</t>
-  </si>
-  <si>
-    <t>vFeYBVCC76mv</t>
-  </si>
-  <si>
-    <t>AMBET123_HALL</t>
-  </si>
-  <si>
-    <t>JJK8wESHxb3M</t>
-  </si>
-  <si>
-    <t>AMBFUN_HALL</t>
-  </si>
-  <si>
-    <t>PK5J10RNLPP9</t>
-  </si>
-  <si>
-    <t>AMBNEWSPORTB</t>
-  </si>
-  <si>
-    <t>opqYIj3u2lON</t>
-  </si>
-  <si>
-    <t>AMBSUPERAPI</t>
-  </si>
-  <si>
-    <t>wMaJIRTy8oaF</t>
-  </si>
-  <si>
-    <t>Ambsuperslot</t>
-  </si>
-  <si>
-    <t>BeJqZOXGqEnr</t>
+    <t>0cmBlC8cky4x</t>
   </si>
   <si>
     <t>AMGOAL_HALL</t>
   </si>
   <si>
-    <t>8eMm3osqQmDW</t>
+    <t>p3MkAmdlrEkc</t>
   </si>
   <si>
     <t>AOA_Hall</t>
   </si>
   <si>
-    <t>47WjDJlIhUP8</t>
+    <t>5PY4VIzpO2t0</t>
   </si>
   <si>
     <t>AQUABET_HALL</t>
   </si>
   <si>
-    <t>gfboHH7DrdDX</t>
-  </si>
-  <si>
-    <t>ARK_HALL</t>
-  </si>
-  <si>
-    <t>TGGO1if8FYBh</t>
+    <t>xDfFolkxPGE0</t>
+  </si>
+  <si>
+    <t>ASIANKING_HALL</t>
+  </si>
+  <si>
+    <t>vxlRqkM2ywK4</t>
   </si>
   <si>
     <t>Askmebet</t>
   </si>
   <si>
-    <t>MK7pGKtPFymI</t>
+    <t>cSUh7kO8Wo4P</t>
   </si>
   <si>
     <t>ATGCLUB888_HALL</t>
   </si>
   <si>
-    <t>wCayFDEB02Ad</t>
+    <t>7zpW8YETdGsy</t>
   </si>
   <si>
     <t>B1NG_HALL</t>
   </si>
   <si>
-    <t>tTK9iAEymmni</t>
-  </si>
-  <si>
-    <t>BBK_HALL</t>
-  </si>
-  <si>
-    <t>ER0tmCl6HpLU</t>
+    <t>L7yIZQQmJ4i2</t>
   </si>
   <si>
     <t>BEIN88_HALL</t>
   </si>
   <si>
-    <t>zSC5YwxS0jhF</t>
+    <t>vjGyQFwuOxBz</t>
   </si>
   <si>
     <t>BEOGAMING_HALL</t>
   </si>
   <si>
-    <t>Q9QWU44xeszR</t>
-  </si>
-  <si>
-    <t>BKK_HALL</t>
-  </si>
-  <si>
-    <t>q3mxb1Y2iPNH</t>
+    <t>fWf9p9d4uvEg</t>
+  </si>
+  <si>
+    <t>BLUEZONE_HALL</t>
+  </si>
+  <si>
+    <t>27d78c0MT6VC</t>
   </si>
   <si>
     <t>BOMA_HALL</t>
   </si>
   <si>
-    <t>jA2RvY8a5jER</t>
+    <t>cX5HT26bGFqr</t>
   </si>
   <si>
     <t>BOSSFU_HALL</t>
   </si>
   <si>
-    <t>xsCSmzJ59s9u</t>
+    <t>UTEJTZLdRjP7</t>
   </si>
   <si>
     <t>BOZZ1688_HALL</t>
   </si>
   <si>
-    <t>yZBdefdH23h6</t>
+    <t>7alGOTRnhnai</t>
   </si>
   <si>
     <t>CLUBBETTO_HALL</t>
   </si>
   <si>
-    <t>9y90KzwMXNiI</t>
-  </si>
-  <si>
-    <t>DASHENG_HALL</t>
-  </si>
-  <si>
-    <t>VkLG8zfvotdN</t>
+    <t>K8w2gOKoxjdB</t>
   </si>
   <si>
     <t>DBG_HALL</t>
   </si>
   <si>
-    <t>JK2gHqiMz0L2</t>
-  </si>
-  <si>
-    <t>DEMO_HALL</t>
-  </si>
-  <si>
-    <t>tIscNHfkDduy</t>
+    <t>pyPm7zoo2fNj</t>
   </si>
   <si>
     <t>DING_HALL</t>
   </si>
   <si>
-    <t>uyNI1Ia8AyQo</t>
+    <t>nSLbs88GXhdb</t>
   </si>
   <si>
     <t>DM_HALL</t>
   </si>
   <si>
-    <t>aD4KPtVUS8Es</t>
+    <t>txQmx23RhAVR</t>
   </si>
   <si>
     <t>DRAGONVIP_HALL</t>
   </si>
   <si>
-    <t>YAz6bo6xXEWz</t>
+    <t>y9kwXpx3gb9X</t>
   </si>
   <si>
     <t>DS_HALL</t>
   </si>
   <si>
-    <t>63m6jCcUPIx0</t>
+    <t>IdLXyJgU87Yi</t>
   </si>
   <si>
     <t>DSSZ_HALL</t>
   </si>
   <si>
-    <t>xCaHIGk1G94m</t>
+    <t>wYbqi55SHMaF</t>
   </si>
   <si>
     <t>DT_HALL</t>
   </si>
   <si>
-    <t>KZZJtD62IPE7</t>
+    <t>us3jrR9MX1io</t>
   </si>
   <si>
     <t>DUMPBET_HALL</t>
   </si>
   <si>
-    <t>VwFwnglwPv2E</t>
+    <t>bG9aq5WRjLTS</t>
   </si>
   <si>
     <t>EBZ_HALL</t>
   </si>
   <si>
-    <t>xdjuIdirbIZK</t>
+    <t>IeBN3ghMD7ny</t>
   </si>
   <si>
     <t>EMC_HALL</t>
   </si>
   <si>
-    <t>tjzoQgM9X8zn</t>
+    <t>fk3QTWeCRCWO</t>
   </si>
   <si>
     <t>ESAN88_HALL</t>
   </si>
   <si>
-    <t>s7GO1FE2ZqFa</t>
+    <t>EaHLUH3ICnQc</t>
   </si>
   <si>
     <t>FASTBET98_HALL</t>
   </si>
   <si>
-    <t>aOF3oRuQrs8H</t>
+    <t>hwlxH06wZZ0O</t>
   </si>
   <si>
     <t>FATCAT_Hall</t>
   </si>
   <si>
-    <t>yprNjnYybLD4</t>
+    <t>qY15gSQ2oW4Y</t>
   </si>
   <si>
     <t>FIN88_HALL</t>
   </si>
   <si>
-    <t>dNWdetnDrlHP</t>
-  </si>
-  <si>
-    <t>FISHDEMO</t>
-  </si>
-  <si>
-    <t>QcA724riUiom</t>
+    <t>Y994nm9v6XGL</t>
   </si>
   <si>
     <t>FOXZ168_HALL</t>
   </si>
   <si>
-    <t>M8AKMGTJqmoY</t>
+    <t>wdArlv5q1l3n</t>
   </si>
   <si>
     <t>FUNKY_HALL</t>
   </si>
   <si>
-    <t>rQy2EPEIDgDZ</t>
+    <t>izA5LJwG8Nxr</t>
   </si>
   <si>
     <t>G2GBET_HALL</t>
   </si>
   <si>
-    <t>B2VHj9SxDrVY</t>
-  </si>
-  <si>
-    <t>GAME1234</t>
-  </si>
-  <si>
-    <t>W0o6JdJB4O8R</t>
+    <t>eSfz5301fM3b</t>
   </si>
   <si>
     <t>GDD_HALL</t>
   </si>
   <si>
-    <t>PotW7wNXjMKb</t>
+    <t>ookLaKxvVrS0</t>
   </si>
   <si>
     <t>GOODDAY88_HALL</t>
   </si>
   <si>
-    <t>KoTvhvIjTaxx</t>
+    <t>JOccOg46H6QY</t>
   </si>
   <si>
     <t>GOTHAM_HALL</t>
   </si>
   <si>
-    <t>H16e8l7P7KN7</t>
+    <t>xFBovlSAki1B</t>
   </si>
   <si>
     <t>GUWIN_HALL</t>
   </si>
   <si>
-    <t>4zIWM5wnBKNy</t>
+    <t>BtwbjDhkCLgv</t>
   </si>
   <si>
     <t>HAFABET_HALL</t>
   </si>
   <si>
-    <t>DoJgrZfnoPIH</t>
+    <t>matH0mErf910</t>
   </si>
   <si>
     <t>HIBIZSOFT_HALL</t>
   </si>
   <si>
-    <t>HObvlducxCTv</t>
-  </si>
-  <si>
-    <t>Hunter3089</t>
-  </si>
-  <si>
-    <t>VkJBV0pZCfxm</t>
-  </si>
-  <si>
-    <t>I8_ROBOT</t>
-  </si>
-  <si>
-    <t>M7B5fNLGWufP</t>
-  </si>
-  <si>
-    <t>iFa_Hall</t>
-  </si>
-  <si>
-    <t>9e7qOBdCwCth</t>
+    <t>d25e8rPFyBO4</t>
+  </si>
+  <si>
+    <t>I8_Hall</t>
+  </si>
+  <si>
+    <t>ClMT0nEm4doY</t>
   </si>
   <si>
     <t>IFM789PLUS_HALL</t>
@@ -492,589 +438,529 @@
     <t>IG_Hall</t>
   </si>
   <si>
-    <t>poOavNVW4TQQ</t>
+    <t>qRO1IpMaWqx0</t>
   </si>
   <si>
     <t>IMPBANKER_HALL</t>
   </si>
   <si>
-    <t>Hare3s9QbaN8</t>
+    <t>OvBf8VKOKM64</t>
   </si>
   <si>
     <t>INWBALL_HALL</t>
   </si>
   <si>
-    <t>AHvLqHYRkN6I</t>
+    <t>9qPeudrvRG1d</t>
   </si>
   <si>
     <t>IPROBET_HALL</t>
   </si>
   <si>
-    <t>y9a9m4cdoI6i</t>
+    <t>laF4w8whwFAk</t>
   </si>
   <si>
     <t>ISB888_HALL</t>
   </si>
   <si>
-    <t>exNKjtthTQWW</t>
+    <t>WtIpRVgRGkaZ</t>
   </si>
   <si>
     <t>IWANTBET_HALL</t>
   </si>
   <si>
-    <t>eM8SVvq4Yl0G</t>
+    <t>xt4XkcZse4es</t>
   </si>
   <si>
     <t>JAMES_HALL</t>
   </si>
   <si>
-    <t>CdR2x8PcJGa1</t>
-  </si>
-  <si>
-    <t>JH_HALL</t>
-  </si>
-  <si>
-    <t>FFrmpi5L5Lpi</t>
-  </si>
-  <si>
-    <t>KBB_HALL</t>
-  </si>
-  <si>
-    <t>0oiM8LClm15L</t>
+    <t>N1atXqMcepSY</t>
   </si>
   <si>
     <t>KG_HALL</t>
   </si>
   <si>
-    <t>iuutoOXRJeQP</t>
+    <t>arVm5I8juY4C</t>
   </si>
   <si>
     <t>KIMBABA_HALL</t>
   </si>
   <si>
-    <t>ZhwqU5b4pwHj</t>
+    <t>3wHm8guOu77l</t>
   </si>
   <si>
     <t>KJ_HALL</t>
   </si>
   <si>
-    <t>T6aTirbKEHEP</t>
+    <t>THojWCiTnqMT</t>
   </si>
   <si>
     <t>KNG365_HALL</t>
   </si>
   <si>
-    <t>F0CF09wBPaGC</t>
+    <t>2PTraMOLJNRt</t>
   </si>
   <si>
     <t>KOBET88_HALL</t>
   </si>
   <si>
-    <t>ayS02iygxWZb</t>
+    <t>Rt2myN9CXhN5</t>
   </si>
   <si>
     <t>Leo_HALL</t>
   </si>
   <si>
-    <t>iPvnJegIdEEM</t>
+    <t>QLOgpt7a8DhO</t>
   </si>
   <si>
     <t>LIVEBET369_HALL</t>
   </si>
   <si>
-    <t>gSJUXkl26qjC</t>
+    <t>aSwNEsbaisAq</t>
   </si>
   <si>
     <t>LUCABET_HALL</t>
   </si>
   <si>
-    <t>86Hfoqn97ie9</t>
+    <t>P3zhkFtC8gHT</t>
   </si>
   <si>
     <t>LUCIABET_HALL</t>
   </si>
   <si>
-    <t>Ym95dV6PplLo</t>
+    <t>A0cC0dWyt1iy</t>
   </si>
   <si>
     <t>LUCKY88_HALL</t>
   </si>
   <si>
-    <t>nEen6TstRy1m</t>
+    <t>wcEIyeyN43bF</t>
   </si>
   <si>
     <t>LUCKYPRO_HALL</t>
   </si>
   <si>
-    <t>n4eR4E8Mtzqh</t>
+    <t>24xKPVE4PqfD</t>
   </si>
   <si>
     <t>LYCAN88_HALL</t>
   </si>
   <si>
-    <t>jiEwKS3QoI4q</t>
+    <t>TFCMkfYzhT7l</t>
   </si>
   <si>
     <t>LYNBET_HALL</t>
   </si>
   <si>
-    <t>SVxItutVDEju</t>
+    <t>tCUfIrV8vpws</t>
   </si>
   <si>
     <t>M4BETS_HALL</t>
   </si>
   <si>
-    <t>TNmBubPU1ipG</t>
+    <t>rDJgpZ0tLP8g</t>
   </si>
   <si>
     <t>MASTER_HALL</t>
   </si>
   <si>
-    <t>F0vBKwHEp5cD</t>
+    <t>TZMZlgNnnRLO</t>
   </si>
   <si>
     <t>MBK168_HALL</t>
   </si>
   <si>
-    <t>QacPWmY6LVhG</t>
+    <t>wcpczs2yj6N2</t>
   </si>
   <si>
     <t>MESSIBET_HALL</t>
   </si>
   <si>
-    <t>0bZnvT7ABrAl</t>
+    <t>mhZST4awgmgJ</t>
   </si>
   <si>
     <t>MGM99WIN_HALL</t>
   </si>
   <si>
-    <t>wikeTLaKjTRX</t>
-  </si>
-  <si>
-    <t>MGP_Hall</t>
-  </si>
-  <si>
-    <t>OlPWQEji38nH</t>
+    <t>L6vTLPsR6fI3</t>
+  </si>
+  <si>
+    <t>MGP_HALL</t>
+  </si>
+  <si>
+    <t>49VORaC18uwm</t>
   </si>
   <si>
     <t>MSCWIN_HALL</t>
   </si>
   <si>
-    <t>mhYndUssSp2v</t>
+    <t>wvxBieXRUfdK</t>
   </si>
   <si>
     <t>MVPATM168_HALL</t>
   </si>
   <si>
-    <t>aAYoymbDCJx1</t>
+    <t>k7xlJONEk7kl</t>
   </si>
   <si>
     <t>MYKJ_HALL</t>
   </si>
   <si>
-    <t>w3R5sanxMUBD</t>
+    <t>2VAskIb2Vivg</t>
   </si>
   <si>
     <t>N88BET_HALL</t>
   </si>
   <si>
-    <t>eiB2KfhlDyB8</t>
+    <t>s8voZGu4po5p</t>
   </si>
   <si>
     <t>NAZA_HALL</t>
   </si>
   <si>
-    <t>MZQ9LzO6j7rR</t>
+    <t>1Xjji5BcthPD</t>
   </si>
   <si>
     <t>NAZAAGENT_HALL</t>
   </si>
   <si>
-    <t>Etx4kaX7nsI4</t>
+    <t>lbDwcaiSysZL</t>
   </si>
   <si>
     <t>NEWSPORTBOOK_HALL</t>
   </si>
   <si>
-    <t>QHZfncBV1vDd</t>
+    <t>BtUkOg8qvSg3</t>
   </si>
   <si>
     <t>NEXOBET_HALL</t>
   </si>
   <si>
-    <t>E6gR10BgUJYu</t>
+    <t>x9j8f5F2NCeh</t>
   </si>
   <si>
     <t>NIGOAL_HALL</t>
   </si>
   <si>
-    <t>k4TNqw0kxV6F</t>
-  </si>
-  <si>
-    <t>testnojp</t>
-  </si>
-  <si>
-    <t>0UdKhhvihAAC</t>
+    <t>5Sr6EwmM1YEG</t>
   </si>
   <si>
     <t>NSA99BET_HALL</t>
   </si>
   <si>
-    <t>HG9vNe4Eqwdi</t>
+    <t>dLQEVLOaIrnA</t>
   </si>
   <si>
     <t>OCMSMUL_HALL</t>
   </si>
   <si>
-    <t>UH1CW5Sz2b3z</t>
+    <t>LooTAyUN2icj</t>
   </si>
   <si>
     <t>OHO999_HALL</t>
   </si>
   <si>
-    <t>xXlYzCdVUXsB</t>
+    <t>ArRTar1WPepZ</t>
   </si>
   <si>
     <t>OMGBET888_HALL</t>
   </si>
   <si>
-    <t>S4PdwBSJD3GQ</t>
+    <t>pEedXp4WbgxE</t>
   </si>
   <si>
     <t>ONECLUBBET_HALL</t>
   </si>
   <si>
-    <t>d6mfNp4mc416</t>
+    <t>so1tWCHpN1eI</t>
   </si>
   <si>
     <t>ONEONEBET_HALL</t>
   </si>
   <si>
-    <t>gSJC1kQCOCJS</t>
+    <t>2c3jtuOSiYgt</t>
   </si>
   <si>
     <t>ONLYWIN_HALL</t>
   </si>
   <si>
-    <t>DnWustCap1IL</t>
+    <t>Ty5TZFiGsVZM</t>
   </si>
   <si>
     <t>PD99BET_HALL</t>
   </si>
   <si>
-    <t>nASAc4PKrO91</t>
-  </si>
-  <si>
-    <t>PG_HALL</t>
-  </si>
-  <si>
-    <t>OBqytzQhppnP</t>
+    <t>d2dsNBbLzDDC</t>
   </si>
   <si>
     <t>POPZA24_HALL</t>
   </si>
   <si>
-    <t>tjRtD54pVVWS</t>
+    <t>QMlcaucfaJvI</t>
   </si>
   <si>
     <t>PREMIER888_HALL</t>
   </si>
   <si>
-    <t>xmry9FjI3Kxq</t>
+    <t>9TbFcUZT8vAJ</t>
   </si>
   <si>
     <t>PV_Hall</t>
   </si>
   <si>
-    <t>mUrAWAjbGUuo</t>
+    <t>2vNUndza793y</t>
   </si>
   <si>
     <t>QIU_HALL</t>
   </si>
   <si>
-    <t>LjrBg5NsejY2</t>
-  </si>
-  <si>
-    <t>QK_Hall</t>
-  </si>
-  <si>
-    <t>dpHRq2WfoV6n</t>
+    <t>oJQucMrjezkj</t>
   </si>
   <si>
     <t>RAPTOR999_HALL</t>
   </si>
   <si>
-    <t>I3M68ka0y1ed</t>
-  </si>
-  <si>
-    <t>ROBOTEST_HALL</t>
-  </si>
-  <si>
-    <t>xAUccoH9WEaz</t>
+    <t>7j9TCjvEKb49</t>
   </si>
   <si>
     <t>ROMANBETS_HALL</t>
   </si>
   <si>
-    <t>9i8HqNE2yfgi</t>
+    <t>xfzl6Prw512x</t>
   </si>
   <si>
     <t>RSG_Hall</t>
   </si>
   <si>
-    <t>okqIFp9pcptM</t>
+    <t>dUrYlRy0GxrM</t>
   </si>
   <si>
     <t>S2KBET_HALL</t>
   </si>
   <si>
-    <t>70Od4BxyO0OA</t>
+    <t>CoMbYcUyJnog</t>
   </si>
   <si>
     <t>SAND1988_HALL</t>
   </si>
   <si>
-    <t>4EJaCjYoc1kA</t>
+    <t>6Yr6tZCgci2e</t>
   </si>
   <si>
     <t>SAND333_HALL</t>
   </si>
   <si>
-    <t>sfT3WIR9rMIZ</t>
+    <t>PVUIbT11Mbn5</t>
   </si>
   <si>
     <t>SB234_HALL</t>
   </si>
   <si>
-    <t>6pVIK7oOe6Az</t>
+    <t>1VLYIbLjMjLw</t>
   </si>
   <si>
     <t>SBOCOPA_HALL</t>
   </si>
   <si>
-    <t>b0WH6hIISgQh</t>
+    <t>HMnMaa3vITOm</t>
   </si>
   <si>
     <t>SCC777_HALL</t>
   </si>
   <si>
-    <t>xtjs5kKiGclS</t>
-  </si>
-  <si>
-    <t>seamless</t>
-  </si>
-  <si>
-    <t>R7F6j7YPO74L</t>
-  </si>
-  <si>
-    <t>singleWallet</t>
-  </si>
-  <si>
-    <t>B96GFE0Ygb03</t>
+    <t>VkPIbY7V9Hkk</t>
   </si>
   <si>
     <t>SKINGBET_HALL</t>
   </si>
   <si>
-    <t>s9Hs3ENjp8QN</t>
+    <t>VqwgmFWMylgd</t>
   </si>
   <si>
     <t>SLOTCITI_Hall</t>
   </si>
   <si>
-    <t>xhDOMjDIBVtW</t>
+    <t>NDEhIuWDDdPT</t>
   </si>
   <si>
     <t>SOJUBET_HALL</t>
   </si>
   <si>
-    <t>9Y4KWCP1hXpm</t>
+    <t>OyozPbiYKtzQ</t>
   </si>
   <si>
     <t>SPIN77_HALL</t>
   </si>
   <si>
-    <t>BxSwj2yTWrub</t>
-  </si>
-  <si>
-    <t>SPORTBOOK88_HALL</t>
-  </si>
-  <si>
-    <t>nZddhy7Ptt4y</t>
+    <t>P4JZl5fybx2l</t>
   </si>
   <si>
     <t>SSC168_HALL</t>
   </si>
   <si>
-    <t>5d8Uf5XtZa0t</t>
-  </si>
-  <si>
-    <t>SUPERGAME99</t>
-  </si>
-  <si>
-    <t>f0rOCU8IokY9</t>
+    <t>flNnY4Oy1lUl</t>
   </si>
   <si>
     <t>TAIPEBET_HALL</t>
   </si>
   <si>
-    <t>NGcUcfyT9IIJ</t>
-  </si>
-  <si>
-    <t>test0707</t>
-  </si>
-  <si>
-    <t>LdxjDNhuxoHj</t>
+    <t>pineYQwd7qii</t>
   </si>
   <si>
     <t>TGO_HALL</t>
   </si>
   <si>
-    <t>UnWIzFJh8wRh</t>
+    <t>GPA14PKEGfyr</t>
   </si>
   <si>
     <t>TH1GAMES_HALL</t>
   </si>
   <si>
-    <t>23n5TM0WLAkw</t>
+    <t>YcVU4gsijc4V</t>
   </si>
   <si>
     <t>THAISPADE_HALL</t>
   </si>
   <si>
-    <t>eFZm15RjMKzn</t>
+    <t>rORnv6sMYgE0</t>
   </si>
   <si>
     <t>TNT911_HALL</t>
   </si>
   <si>
-    <t>PZjhRNJENXUa</t>
+    <t>ZtGJpj3chcOU</t>
   </si>
   <si>
     <t>TP_HALL</t>
   </si>
   <si>
-    <t>GZjZC9WJtkWd</t>
+    <t>jV5F7t3QIraG</t>
   </si>
   <si>
     <t>TT69BET_HALL</t>
   </si>
   <si>
-    <t>q8nCo4wv40Rf</t>
+    <t>Vj1QgIwqKSwQ</t>
+  </si>
+  <si>
+    <t>UBETT_HALL</t>
+  </si>
+  <si>
+    <t>OikgTSuaYNOH</t>
   </si>
   <si>
     <t>UKINGBET_HALL</t>
   </si>
   <si>
-    <t>dN6K63QvAGSS</t>
+    <t>tNlwla0C4md3</t>
   </si>
   <si>
     <t>UPS555_HALL</t>
   </si>
   <si>
-    <t>JuSnXi9o6Egj</t>
+    <t>NSZJTZ5mDoxQ</t>
   </si>
   <si>
     <t>UZIBET_HALL</t>
   </si>
   <si>
-    <t>xETWNjUOnGNg</t>
+    <t>izM0oA5gpARm</t>
   </si>
   <si>
     <t>VA_HALL</t>
   </si>
   <si>
-    <t>Ygzt8S9Itr0B</t>
+    <t>FYgE7cSJMrPm</t>
   </si>
   <si>
     <t>VIEWBET_HALL</t>
   </si>
   <si>
-    <t>ZBY0G9tZRxls</t>
+    <t>np9JzHFglx4E</t>
   </si>
   <si>
     <t>VMAXBET_HALL</t>
   </si>
   <si>
-    <t>oD1sf1IQzDDb</t>
+    <t>7B7twOurBHRy</t>
   </si>
   <si>
     <t>VO_HALL</t>
   </si>
   <si>
-    <t>eagovYXyW7GG</t>
+    <t>5EUIQEDqZB2H</t>
   </si>
   <si>
     <t>VRCBET_HALL</t>
   </si>
   <si>
-    <t>Fe23nI4ZyJb7</t>
+    <t>SsgEXiJrU4MJ</t>
   </si>
   <si>
     <t>WADJAIBET_HALL</t>
   </si>
   <si>
-    <t>MufwhxFW3Tkt</t>
+    <t>Ggi1PjUZtr5H</t>
   </si>
   <si>
     <t>WAW888_HALL</t>
   </si>
   <si>
-    <t>t3bZz4hOSm6P</t>
+    <t>yQeHDm98hBxh</t>
   </si>
   <si>
     <t>WINBETTH_HALL</t>
   </si>
   <si>
-    <t>ygDOi2LRAXnu</t>
+    <t>4beULg9Xgv3m</t>
   </si>
   <si>
     <t>WINGBET_HALL</t>
   </si>
   <si>
-    <t>cQVmscG8yvkV</t>
+    <t>L60DrsrbHOPg</t>
   </si>
   <si>
     <t>WM_HALL</t>
   </si>
   <si>
-    <t>pwkx2Vc0qSWZ</t>
+    <t>QxUJZyyISGQF</t>
   </si>
   <si>
     <t>WM8888_HALL</t>
   </si>
   <si>
-    <t>Lft8tVjkziUG</t>
+    <t>oWXkXCJ0xL4H</t>
   </si>
   <si>
     <t>XMAX999_HALL</t>
   </si>
   <si>
-    <t>y5pWyDhpNFx6</t>
+    <t>8iu7PtztY1wW</t>
   </si>
   <si>
     <t>XYZBET_HALL</t>
   </si>
   <si>
-    <t>Q5VOQwJrp4lm</t>
+    <t>nmEAIch5csno</t>
   </si>
   <si>
     <t>YANG_HALL</t>
   </si>
   <si>
-    <t>xd0HnRhcDq7i</t>
+    <t>kKmVpsKhOwyX</t>
   </si>
   <si>
     <t>YINGBO_HALL</t>
   </si>
   <si>
-    <t>DLZusRrb1X5n</t>
+    <t>Da5HKOHNeeoP</t>
   </si>
   <si>
     <t>ZAMBABET_HALL</t>
   </si>
   <si>
-    <t>ZyodybslRNMo</t>
+    <t>9Pld13Bcu2qz</t>
   </si>
   <si>
     <t>ZH_HALL</t>
@@ -1441,15 +1327,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B176"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD75"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1998,80 +1882,80 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69">
+        <v>131</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="1" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>131</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>154</v>
@@ -2707,158 +2591,6 @@
       </c>
       <c r="B157" s="1" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>